<commit_message>
[BAF510] : 채권 산식 함수 추가 및 par yield 실증
</commit_message>
<xml_diff>
--- a/BAF510채권/hw2/hw2.xlsx
+++ b/BAF510채권/hw2/hw2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20408"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caten\Dropbox\[510] 채권분석\hw_exam_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VSCodeProjects\KAIST_MFE\BAF510채권\hw2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D68EA2-5CEB-4529-9F50-F4E7EB319255}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9253D66B-177B-4634-8CD6-F9CC272B8D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-6765" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>year</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,26 +47,41 @@
     <t>par yield</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>zero/spot</t>
+  </si>
+  <si>
+    <t>discount factor</t>
+  </si>
+  <si>
+    <t>par yield 2</t>
+  </si>
+  <si>
+    <t>zero</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="164" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -85,19 +109,22 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -375,21 +402,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D4A148-0405-491E-A6F8-7A15A4094940}">
-  <dimension ref="A1:H22"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.09765625" customWidth="1"/>
-    <col min="7" max="7" width="12.09765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -399,8 +427,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>0.5</v>
       </c>
@@ -410,9 +447,20 @@
       <c r="C2">
         <v>5.36</v>
       </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="D2" s="3">
+        <f>C2/100</f>
+        <v>5.3600000000000002E-2</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2</f>
+        <v>5.3600000000000002E-2</v>
+      </c>
+      <c r="G2">
+        <f>1/(1+F2)^A2</f>
+        <v>0.97423139106729983</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>1</v>
       </c>
@@ -422,21 +470,29 @@
       <c r="C3">
         <v>5.01</v>
       </c>
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D21" si="0">C3/100</f>
+        <v>5.0099999999999999E-2</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>1.5</v>
       </c>
       <c r="B4">
         <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="E4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>2</v>
       </c>
@@ -445,23 +501,31 @@
       </c>
       <c r="C5">
         <v>4.62</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>4.6199999999999998E-2</v>
       </c>
       <c r="E5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>2.5</v>
       </c>
       <c r="B6">
         <v>5</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="E6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>3</v>
       </c>
@@ -470,45 +534,61 @@
       </c>
       <c r="C7">
         <v>4.42</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>4.4199999999999996E-2</v>
       </c>
       <c r="E7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>3.5</v>
       </c>
       <c r="B8">
         <v>7</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="E8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>4</v>
       </c>
       <c r="B9">
         <v>8</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="E9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>4.5</v>
       </c>
       <c r="B10">
         <v>9</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="E10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>5</v>
       </c>
@@ -517,45 +597,61 @@
       </c>
       <c r="C11">
         <v>4.26</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>4.2599999999999999E-2</v>
       </c>
       <c r="E11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>5.5</v>
       </c>
       <c r="B12">
         <v>11</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="E12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>6</v>
       </c>
       <c r="B13">
         <v>12</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="E13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>6.5</v>
       </c>
       <c r="B14">
         <v>13</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="E14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>7</v>
       </c>
@@ -564,67 +660,91 @@
       </c>
       <c r="C15">
         <v>4.28</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>4.2800000000000005E-2</v>
       </c>
       <c r="E15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>7.5</v>
       </c>
       <c r="B16">
         <v>15</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="E16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>8</v>
       </c>
       <c r="B17">
         <v>16</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="E17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>8.5</v>
       </c>
       <c r="B18">
         <v>17</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="E18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>9</v>
       </c>
       <c r="B19">
         <v>18</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="E19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>9.5</v>
       </c>
       <c r="B20">
         <v>19</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="E20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>10</v>
       </c>
@@ -634,10 +754,146 @@
       <c r="C21">
         <v>4.2699999999999996</v>
       </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>4.2699999999999995E-2</v>
+      </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8">
       <c r="E22" s="1"/>
+    </row>
+    <row r="33" spans="6:11">
+      <c r="F33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <v>0.03</v>
+      </c>
+      <c r="H33">
+        <v>0.05</v>
+      </c>
+      <c r="I33">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J33">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="34" spans="6:11">
+      <c r="F34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34">
+        <f>1/(1+G33)</f>
+        <v>0.970873786407767</v>
+      </c>
+      <c r="H34">
+        <f t="shared" ref="H34:J34" si="1">1/(1+H33)</f>
+        <v>0.95238095238095233</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>0.93457943925233644</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="1"/>
+        <v>0.9174311926605504</v>
+      </c>
+    </row>
+    <row r="37" spans="6:11">
+      <c r="G37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="6:11">
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>3</v>
+      </c>
+      <c r="J38">
+        <v>4</v>
+      </c>
+      <c r="K38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="6:11">
+      <c r="F39">
+        <v>8.5699999999999998E-2</v>
+      </c>
+      <c r="G39">
+        <f>$G$37*$F$39</f>
+        <v>8.57</v>
+      </c>
+      <c r="H39">
+        <f t="shared" ref="H39:I39" si="2">$G$37*$F$39</f>
+        <v>8.57</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="2"/>
+        <v>8.57</v>
+      </c>
+      <c r="J39">
+        <f>F39*G37+G37</f>
+        <v>108.57</v>
+      </c>
+    </row>
+    <row r="40" spans="6:11">
+      <c r="F40">
+        <v>100</v>
+      </c>
+      <c r="G40">
+        <f>G39*(G34)^G38</f>
+        <v>8.3203883495145643</v>
+      </c>
+      <c r="H40">
+        <f t="shared" ref="H40:J40" si="3">H39*(H34)^H38</f>
+        <v>7.7732426303854876</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="3"/>
+        <v>6.9956728049546015</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="3"/>
+        <v>76.913725165348367</v>
+      </c>
+      <c r="K40">
+        <f>SUM(G40:J40)</f>
+        <v>100.00302895020302</v>
+      </c>
+    </row>
+    <row r="41" spans="6:11">
+      <c r="F41" s="3">
+        <f>RATE(4, G39, -F40, G37)</f>
+        <v>8.570000000003386E-2</v>
+      </c>
+      <c r="G41">
+        <f>G39/(1+$F$41)^G38</f>
+        <v>7.8935249148012643</v>
+      </c>
+      <c r="H41">
+        <f t="shared" ref="H41:J41" si="4">H39/(1+$F$41)^H38</f>
+        <v>7.2704475589951363</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="4"/>
+        <v>6.6965529695080672</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="4"/>
+        <v>78.139474556684476</v>
+      </c>
+      <c r="K41">
+        <f>SUM(G41:J41)</f>
+        <v>99.999999999988944</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>